<commit_message>
Add job for csv inventory upload
</commit_message>
<xml_diff>
--- a/failed_rows.xlsx
+++ b/failed_rows.xlsx
@@ -86,6 +86,335 @@
         </is>
       </c>
     </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="0" t="inlineStr">
+        <is>
+          <t>The slug already in use.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>